<commit_message>
typo in pinout XL
</commit_message>
<xml_diff>
--- a/docs/avr64da pinouts.xlsx
+++ b/docs/avr64da pinouts.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB2D446-B6A2-4170-8FAC-A74DB737F8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7137BF1D-C556-4796-940B-762786B24624}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="AVR64DA" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -777,12 +771,6 @@
     <t>VQFN48 TQFP48</t>
   </si>
   <si>
-    <t>VQFN32 TQFP32 SPDIP28</t>
-  </si>
-  <si>
-    <t>SOIC28 SSOP28</t>
-  </si>
-  <si>
     <t>TWIn</t>
   </si>
   <si>
@@ -991,12 +979,18 @@
   </si>
   <si>
     <t>EVOUTA (alt)</t>
+  </si>
+  <si>
+    <t>VQFN32 TQFP32</t>
+  </si>
+  <si>
+    <t>SPDIP28 SOIC28 SSOP28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1179,7 +1173,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1483,44 +1477,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749C9B14-265B-4B59-80C3-AAB9C6447CE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>243</v>
       </c>
@@ -1528,13 +1522,13 @@
         <v>244</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>246</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>248</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>0</v>
@@ -1561,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>8</v>
@@ -1582,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>62</v>
       </c>
@@ -1644,7 +1638,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>63</v>
       </c>
@@ -1706,7 +1700,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>64</v>
       </c>
@@ -1768,7 +1762,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1830,7 +1824,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1865,7 +1859,7 @@
         <v>15</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>156</v>
@@ -1892,7 +1886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -1927,7 +1921,7 @@
         <v>15</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>160</v>
@@ -1954,7 +1948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1989,7 +1983,7 @@
         <v>15</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>165</v>
@@ -2013,10 +2007,10 @@
         <v>15</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -2042,16 +2036,16 @@
         <v>168</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>169</v>
@@ -2072,13 +2066,13 @@
         <v>91</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="T9" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -2134,7 +2128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>7</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>8</v>
       </c>
@@ -2230,7 +2224,7 @@
         <v>15</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>106</v>
@@ -2248,7 +2242,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>9</v>
       </c>
@@ -2288,7 +2282,7 @@
         <v>15</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>139</v>
@@ -2306,7 +2300,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>10</v>
       </c>
@@ -2343,10 +2337,10 @@
         <v>15</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>82</v>
@@ -2364,7 +2358,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>11</v>
       </c>
@@ -2401,10 +2395,10 @@
         <v>15</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>90</v>
@@ -2422,7 +2416,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>12</v>
       </c>
@@ -2453,25 +2447,25 @@
         <v>15</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S16" s="9" t="s">
         <v>15</v>
@@ -2480,7 +2474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>13</v>
       </c>
@@ -2511,16 +2505,16 @@
         <v>15</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N17" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>161</v>
@@ -2529,7 +2523,7 @@
         <v>191</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S17" s="9" t="s">
         <v>15</v>
@@ -2538,7 +2532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>14</v>
       </c>
@@ -2567,13 +2561,13 @@
         <v>15</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="O18" s="9" t="s">
         <v>15</v>
@@ -2585,16 +2579,16 @@
         <v>15</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="S18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="T18" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>15</v>
       </c>
@@ -2623,13 +2617,13 @@
         <v>15</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O19" s="9" t="s">
         <v>15</v>
@@ -2641,16 +2635,16 @@
         <v>15</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T19" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>16</v>
       </c>
@@ -2694,7 +2688,7 @@
         <v>15</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>15</v>
@@ -2712,7 +2706,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>17</v>
       </c>
@@ -2756,13 +2750,13 @@
         <v>15</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="R21" s="9" t="s">
         <v>15</v>
@@ -2774,7 +2768,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>18</v>
       </c>
@@ -2815,10 +2809,10 @@
         <v>207</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>15</v>
@@ -2836,7 +2830,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>19</v>
       </c>
@@ -2877,10 +2871,10 @@
         <v>212</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>15</v>
@@ -2898,7 +2892,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>20</v>
       </c>
@@ -2956,7 +2950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>21</v>
       </c>
@@ -3014,7 +3008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>22</v>
       </c>
@@ -3045,19 +3039,19 @@
         <v>15</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q26" s="9" t="s">
         <v>15</v>
@@ -3072,7 +3066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>23</v>
       </c>
@@ -3103,19 +3097,19 @@
         <v>15</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>15</v>
@@ -3130,7 +3124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>24</v>
       </c>
@@ -3152,7 +3146,7 @@
         <v>15</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>15</v>
@@ -3161,10 +3155,10 @@
         <v>15</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N28" s="9" t="s">
         <v>217</v>
@@ -3173,10 +3167,10 @@
         <v>15</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>15</v>
@@ -3185,10 +3179,10 @@
         <v>15</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>25</v>
       </c>
@@ -3216,13 +3210,13 @@
         <v>15</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="N29" s="9" t="s">
         <v>219</v>
@@ -3240,13 +3234,13 @@
         <v>15</v>
       </c>
       <c r="S29" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="T29" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>26</v>
       </c>
@@ -3290,7 +3284,7 @@
         <v>15</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>15</v>
@@ -3308,7 +3302,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>27</v>
       </c>
@@ -3352,7 +3346,7 @@
         <v>15</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P31" s="9" t="s">
         <v>15</v>
@@ -3370,7 +3364,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>28</v>
       </c>
@@ -3414,7 +3408,7 @@
         <v>15</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>15</v>
@@ -3432,7 +3426,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -3476,7 +3470,7 @@
         <v>15</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>15</v>
@@ -3494,7 +3488,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -3538,7 +3532,7 @@
         <v>15</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>15</v>
@@ -3556,7 +3550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -3600,7 +3594,7 @@
         <v>15</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P35" s="3" t="s">
         <v>15</v>
@@ -3618,7 +3612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -3677,10 +3671,10 @@
         <v>15</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -3718,11 +3712,11 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="T37" s="4"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -3782,7 +3776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -3842,7 +3836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -3880,13 +3874,13 @@
         <v>37</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P40" s="3" t="s">
         <v>15</v>
@@ -3904,7 +3898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -3942,13 +3936,13 @@
         <v>42</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P41" s="3" t="s">
         <v>15</v>
@@ -3966,7 +3960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -4004,13 +3998,13 @@
         <v>47</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N42" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P42" s="3" t="s">
         <v>15</v>
@@ -4028,7 +4022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -4064,13 +4058,13 @@
         <v>53</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="N43" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P43" s="3" t="s">
         <v>15</v>
@@ -4088,7 +4082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -4121,7 +4115,7 @@
         <v>15</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>15</v>
@@ -4130,10 +4124,10 @@
         <v>15</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>15</v>
@@ -4148,7 +4142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41</v>
       </c>
@@ -4181,7 +4175,7 @@
         <v>15</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>15</v>
@@ -4190,10 +4184,10 @@
         <v>15</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>15</v>
@@ -4208,7 +4202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -4241,7 +4235,7 @@
         <v>15</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="M46" s="3" t="s">
         <v>15</v>
@@ -4253,7 +4247,7 @@
         <v>15</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>15</v>
@@ -4268,7 +4262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -4301,7 +4295,7 @@
         <v>66</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M47" s="3" t="s">
         <v>15</v>
@@ -4322,13 +4316,13 @@
         <v>15</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="T47" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -4348,7 +4342,7 @@
         <v>68</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>69</v>
@@ -4370,7 +4364,7 @@
         <v>15</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P48" s="3" t="s">
         <v>15</v>
@@ -4379,7 +4373,7 @@
         <v>15</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S48" s="3" t="s">
         <v>15</v>
@@ -4388,7 +4382,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -4408,7 +4402,7 @@
         <v>73</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>74</v>
@@ -4430,7 +4424,7 @@
         <v>15</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>15</v>
@@ -4439,7 +4433,7 @@
         <v>15</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S49" s="3" t="s">
         <v>15</v>
@@ -4448,7 +4442,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -4468,7 +4462,7 @@
         <v>78</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>79</v>
@@ -4490,7 +4484,7 @@
         <v>81</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>15</v>
@@ -4508,7 +4502,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -4528,7 +4522,7 @@
         <v>78</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>87</v>
@@ -4550,7 +4544,7 @@
         <v>89</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>15</v>
@@ -4568,7 +4562,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -4588,7 +4582,7 @@
         <v>15</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>94</v>
@@ -4610,14 +4604,14 @@
         <v>15</v>
       </c>
       <c r="O52" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="P52" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q52" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="R52" s="3" t="s">
         <v>15</v>
       </c>
@@ -4628,7 +4622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -4648,7 +4642,7 @@
         <v>15</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>98</v>
@@ -4670,14 +4664,14 @@
         <v>15</v>
       </c>
       <c r="O53" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q53" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="P53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q53" s="3" t="s">
-        <v>284</v>
-      </c>
       <c r="R53" s="3" t="s">
         <v>15</v>
       </c>
@@ -4688,7 +4682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -4748,7 +4742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -4808,7 +4802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -4850,10 +4844,10 @@
         <v>15</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>15</v>
@@ -4868,7 +4862,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -4910,10 +4904,10 @@
         <v>15</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>15</v>
@@ -4928,7 +4922,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -4970,10 +4964,10 @@
         <v>15</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q58" s="3" t="s">
         <v>15</v>
@@ -4988,7 +4982,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -5030,10 +5024,10 @@
         <v>15</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>120</v>
@@ -5048,7 +5042,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -5108,7 +5102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -5168,7 +5162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -5201,25 +5195,25 @@
         <v>15</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S62" s="3" t="s">
         <v>15</v>
@@ -5228,7 +5222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -5261,25 +5255,25 @@
         <v>15</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S63" s="3" t="s">
         <v>15</v>
@@ -5288,7 +5282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -5321,10 +5315,10 @@
         <v>15</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>15</v>
@@ -5339,16 +5333,16 @@
         <v>15</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="S64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="T64" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -5381,10 +5375,10 @@
         <v>15</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="N65" s="3" t="s">
         <v>15</v>
@@ -5399,10 +5393,10 @@
         <v>15</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="T65" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
general layout and board sizes
</commit_message>
<xml_diff>
--- a/docs/avr64da pinouts.xlsx
+++ b/docs/avr64da pinouts.xlsx
@@ -347,9 +347,6 @@
     <t>X40/Y40</t>
   </si>
   <si>
-    <t>5, TxD</t>
-  </si>
-  <si>
     <t>WO0</t>
   </si>
   <si>
@@ -985,6 +982,9 @@
   </si>
   <si>
     <t>SPDIP28 SOIC28 SSOP28</t>
+  </si>
+  <si>
+    <t>5,TxD</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1488,8 +1488,8 @@
   <dimension ref="A1:T65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,19 +1516,19 @@
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>244</v>
-      </c>
       <c r="C1" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>316</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>0</v>
@@ -1555,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>8</v>
@@ -1590,52 +1590,52 @@
         <v>22</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1652,52 +1652,52 @@
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1714,7 +1714,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>78</v>
@@ -1723,25 +1723,25 @@
         <v>15</v>
       </c>
       <c r="H4" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>82</v>
@@ -1750,16 +1750,16 @@
         <v>15</v>
       </c>
       <c r="Q4" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="R4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="9" t="s">
+      <c r="T4" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1776,7 +1776,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>78</v>
@@ -1785,25 +1785,25 @@
         <v>15</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>90</v>
@@ -1812,16 +1812,16 @@
         <v>15</v>
       </c>
       <c r="Q5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1838,31 +1838,31 @@
         <v>26</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>15</v>
@@ -1877,7 +1877,7 @@
         <v>15</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>15</v>
@@ -1900,46 +1900,46 @@
         <v>27</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="I7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="N7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>15</v>
@@ -1962,31 +1962,31 @@
         <v>28</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>15</v>
@@ -2007,7 +2007,7 @@
         <v>15</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2024,31 +2024,31 @@
         <v>1</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="M9" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="N9" s="9" t="s">
         <v>15</v>
@@ -2066,7 +2066,7 @@
         <v>91</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="T9" s="10" t="s">
         <v>15</v>
@@ -2080,7 +2080,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>15</v>
@@ -2194,52 +2194,52 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="9" t="s">
+      <c r="M12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T12" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T12" s="10" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2252,52 +2252,52 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="9" t="s">
+      <c r="M13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T13" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T13" s="10" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2310,37 +2310,37 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="I14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="I14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>180</v>
-      </c>
       <c r="M14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>82</v>
@@ -2352,10 +2352,10 @@
         <v>15</v>
       </c>
       <c r="S14" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="T14" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="T14" s="10" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2368,37 +2368,37 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="M15" s="9" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>90</v>
@@ -2413,7 +2413,7 @@
         <v>15</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2426,17 +2426,17 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="I16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2447,25 +2447,25 @@
         <v>15</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S16" s="9" t="s">
         <v>15</v>
@@ -2484,46 +2484,46 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="9" t="s">
+      <c r="I17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q17" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="I17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="R17" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S17" s="9" t="s">
         <v>15</v>
@@ -2540,17 +2540,17 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="I18" s="9" t="s">
         <v>15</v>
       </c>
@@ -2561,13 +2561,13 @@
         <v>15</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O18" s="9" t="s">
         <v>15</v>
@@ -2579,13 +2579,13 @@
         <v>15</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="T18" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2596,17 +2596,17 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="I19" s="9" t="s">
         <v>15</v>
       </c>
@@ -2617,13 +2617,13 @@
         <v>15</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O19" s="9" t="s">
         <v>15</v>
@@ -2635,10 +2635,10 @@
         <v>15</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T19" s="10" t="s">
         <v>15</v>
@@ -2658,52 +2658,52 @@
         <v>2</v>
       </c>
       <c r="E20" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L20" s="9" t="s">
+      <c r="M20" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="N20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="N20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q20" s="9" t="s">
+      <c r="R20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="R20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T20" s="10" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2720,52 +2720,52 @@
         <v>3</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" s="9" t="s">
+      <c r="M21" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="M21" s="9" t="s">
+      <c r="N21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T21" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="R21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T21" s="10" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>78</v>
@@ -2803,31 +2803,31 @@
         <v>15</v>
       </c>
       <c r="L22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="M22" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="N22" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="N22" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S22" s="9" t="s">
+      <c r="T22" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="T22" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2844,7 +2844,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>78</v>
@@ -2865,31 +2865,31 @@
         <v>15</v>
       </c>
       <c r="L23" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="M23" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="N23" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T23" s="10" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>15</v>
@@ -3018,7 +3018,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>15</v>
@@ -3039,19 +3039,19 @@
         <v>15</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q26" s="9" t="s">
         <v>15</v>
@@ -3076,7 +3076,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>15</v>
@@ -3097,19 +3097,19 @@
         <v>15</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>15</v>
@@ -3134,52 +3134,52 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="N28" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="N28" s="9" t="s">
-        <v>217</v>
-      </c>
       <c r="O28" s="9" t="s">
         <v>15</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q28" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T28" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="R28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T28" s="10" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3192,35 +3192,35 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="N29" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="L29" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="M29" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="N29" s="9" t="s">
-        <v>219</v>
-      </c>
       <c r="O29" s="9" t="s">
         <v>15</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>15</v>
       </c>
       <c r="S29" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T29" s="10" t="s">
         <v>15</v>
@@ -3254,52 +3254,52 @@
         <v>6</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="9" t="s">
+      <c r="H30" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="I30" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="J30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T30" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T30" s="10" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3316,52 +3316,52 @@
         <v>7</v>
       </c>
       <c r="E31" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="I31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="9" t="s">
+      <c r="L31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T31" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T31" s="10" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3378,20 +3378,20 @@
         <v>8</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="9" t="s">
+      <c r="H32" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="I32" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>233</v>
-      </c>
       <c r="J32" s="9" t="s">
         <v>15</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>15</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>15</v>
@@ -3423,7 +3423,7 @@
         <v>30</v>
       </c>
       <c r="T32" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3440,52 +3440,52 @@
         <v>9</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="I33" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T33" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T33" s="7" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3514,7 +3514,7 @@
         <v>17</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>15</v>
@@ -3532,7 +3532,7 @@
         <v>15</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>15</v>
@@ -3594,7 +3594,7 @@
         <v>15</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P35" s="3" t="s">
         <v>15</v>
@@ -3638,7 +3638,7 @@
         <v>24</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>25</v>
@@ -3671,7 +3671,7 @@
         <v>15</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
         <v>29</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -3712,7 +3712,7 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T37" s="4"/>
     </row>
@@ -3874,13 +3874,13 @@
         <v>37</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P40" s="3" t="s">
         <v>15</v>
@@ -3936,13 +3936,13 @@
         <v>42</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P41" s="3" t="s">
         <v>15</v>
@@ -3998,13 +3998,13 @@
         <v>47</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N42" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P42" s="3" t="s">
         <v>15</v>
@@ -4058,13 +4058,13 @@
         <v>53</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N43" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P43" s="3" t="s">
         <v>15</v>
@@ -4115,7 +4115,7 @@
         <v>15</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>15</v>
@@ -4124,10 +4124,10 @@
         <v>15</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>15</v>
@@ -4175,7 +4175,7 @@
         <v>15</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>15</v>
@@ -4184,10 +4184,10 @@
         <v>15</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>15</v>
@@ -4235,7 +4235,7 @@
         <v>15</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M46" s="3" t="s">
         <v>15</v>
@@ -4247,7 +4247,7 @@
         <v>15</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>15</v>
@@ -4295,7 +4295,7 @@
         <v>66</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M47" s="3" t="s">
         <v>15</v>
@@ -4316,7 +4316,7 @@
         <v>15</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T47" s="4" t="s">
         <v>15</v>
@@ -4342,7 +4342,7 @@
         <v>68</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>69</v>
@@ -4364,7 +4364,7 @@
         <v>15</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P48" s="3" t="s">
         <v>15</v>
@@ -4373,7 +4373,7 @@
         <v>15</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S48" s="3" t="s">
         <v>15</v>
@@ -4402,7 +4402,7 @@
         <v>73</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>74</v>
@@ -4424,7 +4424,7 @@
         <v>15</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>15</v>
@@ -4433,7 +4433,7 @@
         <v>15</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S49" s="3" t="s">
         <v>15</v>
@@ -4462,7 +4462,7 @@
         <v>78</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>79</v>
@@ -4484,7 +4484,7 @@
         <v>81</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>15</v>
@@ -4522,7 +4522,7 @@
         <v>78</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>87</v>
@@ -4544,7 +4544,7 @@
         <v>89</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>15</v>
@@ -4582,7 +4582,7 @@
         <v>15</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>94</v>
@@ -4604,13 +4604,13 @@
         <v>15</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R52" s="3" t="s">
         <v>15</v>
@@ -4642,7 +4642,7 @@
         <v>15</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>98</v>
@@ -4664,13 +4664,13 @@
         <v>15</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P53" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R53" s="3" t="s">
         <v>15</v>
@@ -4835,7 +4835,7 @@
         <v>15</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>105</v>
+        <v>316</v>
       </c>
       <c r="M56" s="3" t="s">
         <v>15</v>
@@ -4844,10 +4844,10 @@
         <v>15</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>15</v>
@@ -4859,7 +4859,7 @@
         <v>15</v>
       </c>
       <c r="T56" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -4876,16 +4876,16 @@
         <v>15</v>
       </c>
       <c r="E57" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3" t="s">
@@ -4895,31 +4895,31 @@
         <v>15</v>
       </c>
       <c r="L57" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T57" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="M57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O57" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="P57" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T57" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -4936,16 +4936,16 @@
         <v>15</v>
       </c>
       <c r="E58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3" t="s">
@@ -4955,31 +4955,31 @@
         <v>15</v>
       </c>
       <c r="L58" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S58" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S58" s="3" t="s">
+      <c r="T58" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="T58" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -4996,16 +4996,16 @@
         <v>15</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3" t="s">
@@ -5015,31 +5015,31 @@
         <v>15</v>
       </c>
       <c r="L59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q59" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="M59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O59" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="P59" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q59" s="3" t="s">
+      <c r="R59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T59" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="R59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T59" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -5056,7 +5056,7 @@
         <v>20</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>15</v>
@@ -5176,16 +5176,16 @@
         <v>15</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3" t="s">
@@ -5195,25 +5195,25 @@
         <v>15</v>
       </c>
       <c r="L62" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="M62" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="M62" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="N62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S62" s="3" t="s">
         <v>15</v>
@@ -5236,16 +5236,16 @@
         <v>15</v>
       </c>
       <c r="E63" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3" t="s">
@@ -5255,25 +5255,25 @@
         <v>15</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S63" s="3" t="s">
         <v>15</v>
@@ -5296,16 +5296,16 @@
         <v>15</v>
       </c>
       <c r="E64" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3" t="s">
@@ -5315,10 +5315,10 @@
         <v>15</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>15</v>
@@ -5333,13 +5333,13 @@
         <v>15</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="T64" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.35">
@@ -5356,16 +5356,16 @@
         <v>15</v>
       </c>
       <c r="E65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3" t="s">
@@ -5375,10 +5375,10 @@
         <v>15</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N65" s="3" t="s">
         <v>15</v>
@@ -5393,10 +5393,10 @@
         <v>15</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T65" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
added test pads for unused mcu pins
</commit_message>
<xml_diff>
--- a/docs/avr64da pinouts.xlsx
+++ b/docs/avr64da pinouts.xlsx
@@ -326,9 +326,6 @@
     <t>PF5</t>
   </si>
   <si>
-    <t>X37Y37</t>
-  </si>
-  <si>
     <t>2, RxD</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
   </si>
   <si>
     <t>EXTCLK</t>
-  </si>
-  <si>
-    <t>XO/Y0</t>
   </si>
   <si>
     <t>0,TxD</t>
@@ -985,6 +979,12 @@
   </si>
   <si>
     <t>5,TxD</t>
+  </si>
+  <si>
+    <t>X37/Y37</t>
+  </si>
+  <si>
+    <t>X0/Y0</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1487,9 +1487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,19 +1516,19 @@
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>245</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>0</v>
@@ -1555,7 +1555,7 @@
         <v>7</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>8</v>
@@ -1590,52 +1590,52 @@
         <v>22</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="M2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1652,52 +1652,52 @@
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="M3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="9" t="s">
+      <c r="P3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1714,7 +1714,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>78</v>
@@ -1723,25 +1723,25 @@
         <v>15</v>
       </c>
       <c r="H4" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>82</v>
@@ -1750,16 +1750,16 @@
         <v>15</v>
       </c>
       <c r="Q4" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="T4" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1776,7 +1776,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>78</v>
@@ -1785,25 +1785,25 @@
         <v>15</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>90</v>
@@ -1812,7 +1812,7 @@
         <v>15</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>15</v>
@@ -1821,7 +1821,7 @@
         <v>15</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1838,31 +1838,31 @@
         <v>26</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>15</v>
@@ -1877,7 +1877,7 @@
         <v>15</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>15</v>
@@ -1900,46 +1900,46 @@
         <v>27</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="N7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="P7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>15</v>
@@ -1962,31 +1962,31 @@
         <v>28</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>15</v>
@@ -2007,7 +2007,7 @@
         <v>15</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2024,31 +2024,31 @@
         <v>1</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="I9" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="M9" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="N9" s="9" t="s">
         <v>15</v>
@@ -2066,7 +2066,7 @@
         <v>91</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="T9" s="10" t="s">
         <v>15</v>
@@ -2080,7 +2080,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>15</v>
@@ -2194,52 +2194,52 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="M12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T12" s="10" t="s">
         <v>170</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T12" s="10" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2252,52 +2252,52 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="M13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T13" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T13" s="10" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2310,37 +2310,37 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>179</v>
-      </c>
       <c r="M14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>82</v>
@@ -2352,10 +2352,10 @@
         <v>15</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="T14" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2368,37 +2368,37 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>184</v>
-      </c>
       <c r="M15" s="9" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>90</v>
@@ -2413,7 +2413,7 @@
         <v>15</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>15</v>
@@ -2435,7 +2435,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>15</v>
@@ -2447,25 +2447,25 @@
         <v>15</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N16" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="S16" s="9" t="s">
         <v>15</v>
@@ -2484,46 +2484,46 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q17" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>190</v>
-      </c>
       <c r="R17" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S17" s="9" t="s">
         <v>15</v>
@@ -2540,7 +2540,7 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>15</v>
@@ -2549,7 +2549,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>15</v>
@@ -2561,13 +2561,13 @@
         <v>15</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="O18" s="9" t="s">
         <v>15</v>
@@ -2579,13 +2579,13 @@
         <v>15</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="T18" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>15</v>
@@ -2605,7 +2605,7 @@
         <v>15</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>15</v>
@@ -2617,13 +2617,13 @@
         <v>15</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O19" s="9" t="s">
         <v>15</v>
@@ -2635,10 +2635,10 @@
         <v>15</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="T19" s="10" t="s">
         <v>15</v>
@@ -2658,52 +2658,52 @@
         <v>2</v>
       </c>
       <c r="E20" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="M20" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L20" s="9" t="s">
+      <c r="N20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="R20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" s="10" t="s">
         <v>197</v>
-      </c>
-      <c r="N20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="R20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T20" s="10" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2720,52 +2720,52 @@
         <v>3</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="M21" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" s="9" t="s">
+      <c r="N21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T21" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="R21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T21" s="10" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>78</v>
@@ -2803,31 +2803,31 @@
         <v>15</v>
       </c>
       <c r="L22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="T22" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S22" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="T22" s="10" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2844,7 +2844,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>78</v>
@@ -2865,31 +2865,31 @@
         <v>15</v>
       </c>
       <c r="L23" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="M23" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="P23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T23" s="10" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>15</v>
@@ -3018,7 +3018,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>15</v>
@@ -3039,19 +3039,19 @@
         <v>15</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q26" s="9" t="s">
         <v>15</v>
@@ -3076,7 +3076,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>15</v>
@@ -3097,19 +3097,19 @@
         <v>15</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q27" s="9" t="s">
         <v>15</v>
@@ -3134,7 +3134,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>15</v>
@@ -3146,7 +3146,7 @@
         <v>15</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>15</v>
@@ -3155,22 +3155,22 @@
         <v>15</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O28" s="9" t="s">
         <v>15</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>15</v>
@@ -3179,7 +3179,7 @@
         <v>15</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3192,7 +3192,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>15</v>
@@ -3210,16 +3210,16 @@
         <v>15</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O29" s="9" t="s">
         <v>15</v>
@@ -3234,7 +3234,7 @@
         <v>15</v>
       </c>
       <c r="S29" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="T29" s="10" t="s">
         <v>15</v>
@@ -3254,52 +3254,52 @@
         <v>6</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="9" t="s">
+      <c r="I30" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="J30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T30" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="P30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T30" s="10" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3316,52 +3316,52 @@
         <v>7</v>
       </c>
       <c r="E31" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="9" t="s">
+      <c r="I31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="L31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T31" s="10" t="s">
         <v>226</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="T31" s="10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3378,20 +3378,20 @@
         <v>8</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="9" t="s">
+      <c r="I32" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>232</v>
-      </c>
       <c r="J32" s="9" t="s">
         <v>15</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>15</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>15</v>
@@ -3423,7 +3423,7 @@
         <v>30</v>
       </c>
       <c r="T32" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3440,52 +3440,52 @@
         <v>9</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="6" t="s">
+      <c r="I33" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T33" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T33" s="7" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -3514,7 +3514,7 @@
         <v>17</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>15</v>
@@ -3532,7 +3532,7 @@
         <v>15</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>15</v>
@@ -3594,7 +3594,7 @@
         <v>15</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P35" s="3" t="s">
         <v>15</v>
@@ -3638,7 +3638,7 @@
         <v>24</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>25</v>
@@ -3671,10 +3671,10 @@
         <v>15</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>29</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -3712,7 +3712,7 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="T37" s="4"/>
     </row>
@@ -3874,13 +3874,13 @@
         <v>37</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P40" s="3" t="s">
         <v>15</v>
@@ -3936,13 +3936,13 @@
         <v>42</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="P41" s="3" t="s">
         <v>15</v>
@@ -3998,13 +3998,13 @@
         <v>47</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="N42" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P42" s="3" t="s">
         <v>15</v>
@@ -4058,13 +4058,13 @@
         <v>53</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N43" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P43" s="3" t="s">
         <v>15</v>
@@ -4115,7 +4115,7 @@
         <v>15</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>15</v>
@@ -4124,10 +4124,10 @@
         <v>15</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>15</v>
@@ -4175,7 +4175,7 @@
         <v>15</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>15</v>
@@ -4184,10 +4184,10 @@
         <v>15</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>15</v>
@@ -4235,7 +4235,7 @@
         <v>15</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M46" s="3" t="s">
         <v>15</v>
@@ -4247,7 +4247,7 @@
         <v>15</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>15</v>
@@ -4295,7 +4295,7 @@
         <v>66</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M47" s="3" t="s">
         <v>15</v>
@@ -4316,7 +4316,7 @@
         <v>15</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="T47" s="4" t="s">
         <v>15</v>
@@ -4342,7 +4342,7 @@
         <v>68</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>69</v>
@@ -4364,7 +4364,7 @@
         <v>15</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P48" s="3" t="s">
         <v>15</v>
@@ -4373,7 +4373,7 @@
         <v>15</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="S48" s="3" t="s">
         <v>15</v>
@@ -4402,7 +4402,7 @@
         <v>73</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>74</v>
@@ -4424,7 +4424,7 @@
         <v>15</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>15</v>
@@ -4433,7 +4433,7 @@
         <v>15</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S49" s="3" t="s">
         <v>15</v>
@@ -4462,7 +4462,7 @@
         <v>78</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>79</v>
@@ -4484,7 +4484,7 @@
         <v>81</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>15</v>
@@ -4522,7 +4522,7 @@
         <v>78</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>87</v>
@@ -4544,7 +4544,7 @@
         <v>89</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>15</v>
@@ -4582,7 +4582,7 @@
         <v>15</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>94</v>
@@ -4604,13 +4604,13 @@
         <v>15</v>
       </c>
       <c r="O52" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="P52" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q52" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="R52" s="3" t="s">
         <v>15</v>
@@ -4642,10 +4642,10 @@
         <v>15</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>98</v>
+        <v>315</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3" t="s">
@@ -4655,7 +4655,7 @@
         <v>15</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M53" s="3" t="s">
         <v>15</v>
@@ -4664,13 +4664,13 @@
         <v>15</v>
       </c>
       <c r="O53" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q53" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="P53" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q53" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="R53" s="3" t="s">
         <v>15</v>
@@ -4696,10 +4696,10 @@
         <v>18</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>15</v>
@@ -4756,7 +4756,7 @@
         <v>19</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>15</v>
@@ -4816,16 +4816,16 @@
         <v>15</v>
       </c>
       <c r="E56" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3" t="s">
@@ -4835,7 +4835,7 @@
         <v>15</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M56" s="3" t="s">
         <v>15</v>
@@ -4844,10 +4844,10 @@
         <v>15</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>15</v>
@@ -4859,7 +4859,7 @@
         <v>15</v>
       </c>
       <c r="T56" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -4876,16 +4876,16 @@
         <v>15</v>
       </c>
       <c r="E57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3" t="s">
@@ -4895,31 +4895,31 @@
         <v>15</v>
       </c>
       <c r="L57" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T57" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="M57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O57" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="P57" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T57" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -4936,16 +4936,16 @@
         <v>15</v>
       </c>
       <c r="E58" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3" t="s">
@@ -4955,31 +4955,31 @@
         <v>15</v>
       </c>
       <c r="L58" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S58" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="M58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S58" s="3" t="s">
+      <c r="T58" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="T58" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -4996,16 +4996,16 @@
         <v>15</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3" t="s">
@@ -5015,31 +5015,31 @@
         <v>15</v>
       </c>
       <c r="L59" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q59" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="M59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O59" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="P59" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q59" s="3" t="s">
+      <c r="R59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T59" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="R59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T59" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -5056,7 +5056,7 @@
         <v>20</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>15</v>
@@ -5176,16 +5176,16 @@
         <v>15</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3" t="s">
@@ -5195,25 +5195,25 @@
         <v>15</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q62" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R62" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="S62" s="3" t="s">
         <v>15</v>
@@ -5236,16 +5236,16 @@
         <v>15</v>
       </c>
       <c r="E63" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3" t="s">
@@ -5255,25 +5255,25 @@
         <v>15</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S63" s="3" t="s">
         <v>15</v>
@@ -5296,16 +5296,16 @@
         <v>15</v>
       </c>
       <c r="E64" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3" t="s">
@@ -5315,10 +5315,10 @@
         <v>15</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>15</v>
@@ -5333,13 +5333,13 @@
         <v>15</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="T64" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.35">
@@ -5356,16 +5356,16 @@
         <v>15</v>
       </c>
       <c r="E65" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3" t="s">
@@ -5375,10 +5375,10 @@
         <v>15</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N65" s="3" t="s">
         <v>15</v>
@@ -5393,10 +5393,10 @@
         <v>15</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="T65" s="4" t="s">
         <v>15</v>

</xml_diff>